<commit_message>
add README and make minor changes
</commit_message>
<xml_diff>
--- a/quantteaching.xlsx
+++ b/quantteaching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egl/Dropbox/web/GitHub/qted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CB9C90-55E4-7B49-9EF1-BA90551520F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD10E7D-FAB3-E640-B65F-FF4E5A397E6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{04BA067E-096B-8644-8CC0-269C7F9ACFCF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Perception</t>
+  </si>
+  <si>
+    <t>revised</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C04EB78-B9FB-6747-8407-380268F9A751}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,7 +496,7 @@
     <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +530,11 @@
       <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -557,8 +563,11 @@
         <v>11</v>
       </c>
       <c r="K2" s="2"/>
+      <c r="L2">
+        <v>20181202</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -583,8 +592,11 @@
       <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="L3">
+        <v>20181202</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -608,6 +620,9 @@
       </c>
       <c r="J4" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="L4">
+        <v>20181202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add example on IE users and IQ
</commit_message>
<xml_diff>
--- a/quantteaching.xlsx
+++ b/quantteaching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egl/Dropbox/web/GitHub/qted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD10E7D-FAB3-E640-B65F-FF4E5A397E6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368613F2-28ED-674E-BD3F-6447F6EDA130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{04BA067E-096B-8644-8CC0-269C7F9ACFCF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -115,6 +115,27 @@
   </si>
   <si>
     <t>revised</t>
+  </si>
+  <si>
+    <t>https://www.macmillanihe.com/companion/De-Vries-Critical-Statistics/</t>
+  </si>
+  <si>
+    <t>IE Users Have Lower IQ Than Users of Other Web Browsers [STUDY]</t>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>IQ</t>
+  </si>
+  <si>
+    <t>technology, intelligence</t>
+  </si>
+  <si>
+    <t>web browser</t>
+  </si>
+  <si>
+    <t>https://mashable.com/2011/07/29/internet-explorer-iq/</t>
   </si>
 </sst>
 </file>
@@ -485,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C04EB78-B9FB-6747-8407-380268F9A751}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,11 +646,45 @@
         <v>20181202</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>2017</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>20181202</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{6FA86626-E827-1D4B-8F5B-B654676403B7}"/>
     <hyperlink ref="J4" r:id="rId2" xr:uid="{D0585865-2122-BE44-B5AB-253083BD673E}"/>
     <hyperlink ref="J3" r:id="rId3" xr:uid="{685353C5-B1C0-2E4A-9A54-AED1334E9CD3}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{9C9B24B1-6FAE-924F-972A-392669951580}"/>
+    <hyperlink ref="J5" r:id="rId5" xr:uid="{F71890FE-F2AC-4246-AA48-D14893216896}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add example with 'Another Benefit to Going to Museums'
</commit_message>
<xml_diff>
--- a/quantteaching.xlsx
+++ b/quantteaching.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egl/Dropbox/web/GitHub/qted/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/qted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368613F2-28ED-674E-BD3F-6447F6EDA130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D637C70-C9D3-6247-96B3-E437E3CBF907}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{04BA067E-096B-8644-8CC0-269C7F9ACFCF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t>https://mashable.com/2011/07/29/internet-explorer-iq/</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2019/12/22/us/arts-health-effects-ucl-study.html</t>
+  </si>
+  <si>
+    <t>Another Benefit to Going to Museums? You May Live Longer</t>
+  </si>
+  <si>
+    <t>Mortality</t>
+  </si>
+  <si>
+    <t>Museum attendance</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>correlation, causation</t>
+  </si>
+  <si>
+    <t>culture, health</t>
   </si>
 </sst>
 </file>
@@ -193,7 +214,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -210,7 +231,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -506,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C04EB78-B9FB-6747-8407-380268F9A751}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,6 +699,38 @@
         <v>20181202</v>
       </c>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>2019</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6">
+        <v>20191225</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{6FA86626-E827-1D4B-8F5B-B654676403B7}"/>
@@ -685,6 +738,7 @@
     <hyperlink ref="J3" r:id="rId3" xr:uid="{685353C5-B1C0-2E4A-9A54-AED1334E9CD3}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{9C9B24B1-6FAE-924F-972A-392669951580}"/>
     <hyperlink ref="J5" r:id="rId5" xr:uid="{F71890FE-F2AC-4246-AA48-D14893216896}"/>
+    <hyperlink ref="J6" r:id="rId6" xr:uid="{BB03E33A-2784-D143-9784-8CCC9F4FD2E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>